<commit_message>
Improved readability in refactoring metrics raport
</commit_message>
<xml_diff>
--- a/docs/refactoring/gatewayController- refactoring metrics.xlsx
+++ b/docs/refactoring/gatewayController- refactoring metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\rowing app\SEM34c\docs\refactoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A5E9559-DE2F-4A5F-88DF-47DC1ECF74F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD8215E-923B-4678-9B8D-58C21E58CEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E6CB794-808F-4F48-AFB2-A6D83001908A}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>low-medium</t>
   </si>
   <si>
-    <t>After:</t>
-  </si>
-  <si>
     <t>nl.tudelft.sem.template.gateway.controllers.GatewayActivityMatchController</t>
   </si>
   <si>
@@ -146,7 +143,10 @@
     <t>GatewayAuthenticationController</t>
   </si>
   <si>
-    <t>Before:</t>
+    <t>Before refactoring:</t>
+  </si>
+  <si>
+    <t>After refactoring:</t>
   </si>
 </sst>
 </file>
@@ -162,12 +162,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,8 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,12 +522,12 @@
   <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -533,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
@@ -617,16 +638,16 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G3">
@@ -686,7 +707,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
@@ -765,21 +786,21 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G10">
@@ -839,21 +860,21 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G11">
@@ -913,21 +934,21 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G12">
@@ -992,16 +1013,16 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G13">
@@ -1061,5 +1082,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>